<commit_message>
MaJ planning + add docu ui ux
</commit_message>
<xml_diff>
--- a/PROJET FIL ROUGE/Historique des taches.xlsx
+++ b/PROJET FIL ROUGE/Historique des taches.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julie\Desktop\ADRAR Formation Dev\PROJET FIL ROUGE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julien\Desktop\Cours\PROJET FIL ROUGE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE42B9AF-6C9B-4D7F-972C-BC3AC1C5E96A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="4815" windowWidth="38640" windowHeight="21120" xr2:uid="{3E0017A0-76FB-4A8B-971A-4A0FC8F145F2}"/>
+    <workbookView xWindow="-38520" yWindow="4815" windowWidth="38640" windowHeight="21120"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,18 +34,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Planning Projet fil Rouge Maison Jonis</t>
   </si>
   <si>
     <t>Commencer le CDC, maquette, charte graphique et arborescence</t>
   </si>
+  <si>
+    <t>Finition de la partie intro du CDC</t>
+  </si>
+  <si>
+    <t>Mockup Fini</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -392,26 +397,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABF870B8-F5A9-4F5C-980B-C6BF91C949E9}">
-  <dimension ref="C5:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C5:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <v>45240</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="1">
+        <v>45241</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="1">
+        <v>45245</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update projet fil rouge
</commit_message>
<xml_diff>
--- a/PROJET FIL ROUGE/Historique des taches.xlsx
+++ b/PROJET FIL ROUGE/Historique des taches.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julien\Desktop\Cours\PROJET FIL ROUGE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julie\Desktop\ADRAR Formation Dev\PROJET FIL ROUGE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F0291C-5FD9-4DA6-95B3-B873429A9829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="4815" windowWidth="38640" windowHeight="21120"/>
+    <workbookView xWindow="-38520" yWindow="4815" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -19,22 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Planning Projet fil Rouge Maison Jonis</t>
   </si>
@@ -47,11 +38,14 @@
   <si>
     <t>Mockup Fini</t>
   </si>
+  <si>
+    <t>Poursuite du CDC, charte graph, moodboard, arbo</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -397,21 +391,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C5:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C9" s="1">
         <v>45240</v>
       </c>
@@ -419,10 +413,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C11" s="1">
         <v>45241</v>
       </c>
@@ -430,12 +424,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C13" s="1">
         <v>45245</v>
       </c>
       <c r="E13" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C15" s="1">
+        <v>45250</v>
+      </c>
+      <c r="E15" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pydéfis et fil rouge
</commit_message>
<xml_diff>
--- a/PROJET FIL ROUGE/Historique des taches.xlsx
+++ b/PROJET FIL ROUGE/Historique des taches.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julie\Desktop\ADRAR Formation Dev\PROJET FIL ROUGE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F0291C-5FD9-4DA6-95B3-B873429A9829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6D83CC-092C-4984-8F3B-2DED6BA057B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="4815" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32880" yWindow="8865" windowWidth="28800" windowHeight="15375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Planning Projet fil Rouge Maison Jonis</t>
   </si>
@@ -36,10 +36,25 @@
     <t>Finition de la partie intro du CDC</t>
   </si>
   <si>
-    <t>Mockup Fini</t>
-  </si>
-  <si>
     <t>Poursuite du CDC, charte graph, moodboard, arbo</t>
+  </si>
+  <si>
+    <t>Début du prototype</t>
+  </si>
+  <si>
+    <t>Poursuite proto</t>
+  </si>
+  <si>
+    <t>Zoning Fini</t>
+  </si>
+  <si>
+    <t>Moodboard/arborescence/wireframe terminés</t>
+  </si>
+  <si>
+    <t>Prototype terminé</t>
+  </si>
+  <si>
+    <t>Diagramme de gant / mockup</t>
   </si>
 </sst>
 </file>
@@ -392,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C5:E15"/>
+  <dimension ref="C5:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -421,7 +436,7 @@
         <v>45241</v>
       </c>
       <c r="E11" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.35">
@@ -437,7 +452,47 @@
         <v>45250</v>
       </c>
       <c r="E15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C17" s="1">
+        <v>45255</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C19" s="1">
+        <v>45256</v>
+      </c>
+      <c r="E19" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C21" s="1">
+        <v>45258</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C23" s="1">
+        <v>45259</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C25" s="1">
+        <v>45263</v>
+      </c>
+      <c r="E25" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>